<commit_message>
bugs on single block exceptions
</commit_message>
<xml_diff>
--- a/Gabari/output/test/output.xlsx
+++ b/Gabari/output/test/output.xlsx
@@ -13,7 +13,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="28">
   <si>
     <t>مبدا</t>
   </si>
@@ -70,6 +70,33 @@
   </si>
   <si>
     <t>قابل عبور</t>
+  </si>
+  <si>
+    <t>بهرام - رباط کریم</t>
+  </si>
+  <si>
+    <t>گاباری 5.4</t>
+  </si>
+  <si>
+    <t>رباط کریم - جدایش</t>
+  </si>
+  <si>
+    <t>گاباری 4.9</t>
+  </si>
+  <si>
+    <t>جدایش - باغ یک</t>
+  </si>
+  <si>
+    <t>باغ یک - سواریان</t>
+  </si>
+  <si>
+    <t>سواریان - نورآباد</t>
+  </si>
+  <si>
+    <t>نورآباد - بندرامام خمینی</t>
+  </si>
+  <si>
+    <t>گاباری ۴.۷</t>
   </si>
 </sst>
 </file>
@@ -77,13 +104,43 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="0"/>
-  <fonts count="3">
+  <fonts count="9">
     <font>
       <sz val="11.0"/>
       <color indexed="8"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <name val="B Zar"/>
+      <sz val="11.0"/>
+      <charset val="178"/>
+    </font>
+    <font>
+      <name val="B Zar"/>
+      <sz val="11.0"/>
+      <charset val="178"/>
+    </font>
+    <font>
+      <name val="B Zar"/>
+      <sz val="11.0"/>
+      <charset val="178"/>
+    </font>
+    <font>
+      <name val="B Zar"/>
+      <sz val="11.0"/>
+      <charset val="178"/>
+    </font>
+    <font>
+      <name val="B Zar"/>
+      <sz val="11.0"/>
+      <charset val="178"/>
+    </font>
+    <font>
+      <name val="B Zar"/>
+      <sz val="11.0"/>
+      <charset val="178"/>
     </font>
     <font>
       <name val="B Zar"/>
@@ -147,12 +204,30 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="3" fontId="1" fillId="3" borderId="4" xfId="0" applyFont="true" applyNumberFormat="true" applyFill="true" applyBorder="true">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="3" fontId="2" fillId="4" borderId="4" xfId="0" applyFont="true" applyNumberFormat="true" applyFill="true" applyBorder="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="3" fontId="3" fillId="4" borderId="4" xfId="0" applyFont="true" applyNumberFormat="true" applyFill="true" applyBorder="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="3" fontId="4" fillId="4" borderId="4" xfId="0" applyFont="true" applyNumberFormat="true" applyFill="true" applyBorder="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="3" fontId="5" fillId="4" borderId="4" xfId="0" applyFont="true" applyNumberFormat="true" applyFill="true" applyBorder="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="3" fontId="6" fillId="4" borderId="4" xfId="0" applyFont="true" applyNumberFormat="true" applyFill="true" applyBorder="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="3" fontId="7" fillId="4" borderId="4" xfId="0" applyFont="true" applyNumberFormat="true" applyFill="true" applyBorder="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="3" fontId="8" fillId="4" borderId="4" xfId="0" applyFont="true" applyNumberFormat="true" applyFill="true" applyBorder="true">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -167,8 +242,8 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.0"/>
   <cols>
-    <col min="1" max="1" customWidth="true" width="21.0" collapsed="false"/>
-    <col min="2" max="2" customWidth="true" width="21.0" collapsed="false"/>
+    <col min="1" max="1" customWidth="true" width="21.0" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" width="21.0" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -250,18 +325,18 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:F2"/>
+  <dimension ref="A1:F8"/>
   <sheetViews>
     <sheetView workbookViewId="0" rightToLeft="true"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.0"/>
   <cols>
-    <col min="1" max="1" customWidth="true" width="21.0" collapsed="false"/>
-    <col min="2" max="2" customWidth="true" width="21.0" collapsed="false"/>
-    <col min="3" max="3" customWidth="true" width="21.0" collapsed="false"/>
-    <col min="4" max="4" customWidth="true" width="21.0" collapsed="false"/>
-    <col min="5" max="5" customWidth="true" width="21.0" collapsed="false"/>
-    <col min="6" max="6" customWidth="true" width="21.0" collapsed="false"/>
+    <col min="1" max="1" customWidth="true" width="21.0" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" width="21.0" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" width="21.0" collapsed="true"/>
+    <col min="4" max="4" customWidth="true" width="21.0" collapsed="true"/>
+    <col min="5" max="5" customWidth="true" width="21.0" collapsed="true"/>
+    <col min="6" max="6" customWidth="true" width="21.0" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -304,6 +379,126 @@
         <v>0.0</v>
       </c>
     </row>
+    <row r="3">
+      <c r="A3" t="s" s="3">
+        <v>19</v>
+      </c>
+      <c r="B3" t="s" s="3">
+        <v>20</v>
+      </c>
+      <c r="C3" t="s" s="3">
+        <v>17</v>
+      </c>
+      <c r="D3" t="n" s="3">
+        <v>25.0</v>
+      </c>
+      <c r="E3" t="s" s="3">
+        <v>18</v>
+      </c>
+      <c r="F3" t="n" s="3">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="s" s="4">
+        <v>21</v>
+      </c>
+      <c r="B4" t="s" s="4">
+        <v>22</v>
+      </c>
+      <c r="C4" t="s" s="4">
+        <v>17</v>
+      </c>
+      <c r="D4" t="n" s="4">
+        <v>304.138126514911</v>
+      </c>
+      <c r="E4" t="s" s="4">
+        <v>18</v>
+      </c>
+      <c r="F4" t="n" s="4">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="s" s="5">
+        <v>23</v>
+      </c>
+      <c r="B5" t="s" s="5">
+        <v>20</v>
+      </c>
+      <c r="C5" t="s" s="5">
+        <v>17</v>
+      </c>
+      <c r="D5" t="n" s="5">
+        <v>25.0</v>
+      </c>
+      <c r="E5" t="s" s="5">
+        <v>18</v>
+      </c>
+      <c r="F5" t="n" s="5">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="s" s="6">
+        <v>24</v>
+      </c>
+      <c r="B6" t="s" s="6">
+        <v>16</v>
+      </c>
+      <c r="C6" t="s" s="6">
+        <v>17</v>
+      </c>
+      <c r="D6" t="n" s="6">
+        <v>35.35533905932738</v>
+      </c>
+      <c r="E6" t="s" s="6">
+        <v>18</v>
+      </c>
+      <c r="F6" t="n" s="6">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="s" s="7">
+        <v>25</v>
+      </c>
+      <c r="B7" t="s" s="7">
+        <v>20</v>
+      </c>
+      <c r="C7" t="s" s="7">
+        <v>17</v>
+      </c>
+      <c r="D7" t="n" s="7">
+        <v>25.0</v>
+      </c>
+      <c r="E7" t="s" s="7">
+        <v>18</v>
+      </c>
+      <c r="F7" t="n" s="7">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="s" s="8">
+        <v>26</v>
+      </c>
+      <c r="B8" t="s" s="8">
+        <v>27</v>
+      </c>
+      <c r="C8" t="s" s="8">
+        <v>17</v>
+      </c>
+      <c r="D8" t="n" s="8">
+        <v>335.4101966249685</v>
+      </c>
+      <c r="E8" t="s" s="8">
+        <v>17</v>
+      </c>
+      <c r="F8" t="n" s="8">
+        <v>100.0</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>

</xml_diff>